<commit_message>
I changed all the features within
</commit_message>
<xml_diff>
--- a/buyer_data.xlsx
+++ b/buyer_data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,44 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCCCC"/>
+        <bgColor rgb="00FFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002F4F4F"/>
+        <bgColor rgb="002F4F4F"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +77,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,19 +463,79 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Buyer ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Items Ordered</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Apple Juice: 5pcs., Manggo Juice: 1pcs., Guyabano Juice: 1pcs.</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>PHP 140.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Guyabano Juice: 2pcs., Ice Mixed Guyabano with Teal: 4pcs., Manggo Juice: 1pcs.</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>PHP 180.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Apple Juice: 3pcs.</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>PHP 60.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Ice Mixed Guyabano with Teal: 3pcs., Manggo Juice: 3pcs., Guyabano Juice: 1pcs.</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>PHP 170.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
I added an option for the user to remove items from the cart, to clear out items from the cart at once.
</commit_message>
<xml_diff>
--- a/buyer_data.xlsx
+++ b/buyer_data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,44 +25,13 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ADD8E6"/>
-        <bgColor rgb="00ADD8E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D3D3D3"/>
-        <bgColor rgb="00D3D3D3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFCCCC"/>
-        <bgColor rgb="00FFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="002F4F4F"/>
-        <bgColor rgb="002F4F4F"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,18 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -454,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,79 +422,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Buyer ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Items Ordered</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
-          <t>Apple Juice: 5pcs., Manggo Juice: 1pcs., Guyabano Juice: 1pcs.</t>
+          <t>Apple Juice: 5pcs.</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
-          <t>PHP 140.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Guyabano Juice: 2pcs., Ice Mixed Guyabano with Teal: 4pcs., Manggo Juice: 1pcs.</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>PHP 180.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Apple Juice: 3pcs.</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>PHP 60.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Ice Mixed Guyabano with Teal: 3pcs., Manggo Juice: 3pcs., Guyabano Juice: 1pcs.</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>PHP 170.00</t>
+          <t>PHP 100.00</t>
         </is>
       </c>
     </row>

</xml_diff>